<commit_message>
add withdraw excel_test_case code
</commit_message>
<xml_diff>
--- a/datas/user_test.xlsx
+++ b/datas/user_test.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python_workspace\api-test\datas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9345" activeTab="3"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9345" windowWidth="23040" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="register" sheetId="1" r:id="rId1"/>
-    <sheet name="login" sheetId="2" r:id="rId2"/>
-    <sheet name="recharge" sheetId="3" r:id="rId3"/>
-    <sheet name="withdraw" sheetId="4" r:id="rId4"/>
-    <sheet name="list" sheetId="5" r:id="rId5"/>
-    <sheet name="bidLoan" sheetId="6" r:id="rId6"/>
-    <sheet name="init" sheetId="7" r:id="rId7"/>
+    <sheet name="register" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="login" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="recharge" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="withdraw" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="list" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="bidLoan" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="init" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="140">
   <si>
     <t>caseId</t>
   </si>
@@ -318,627 +313,237 @@
     <t>{'status': 1, 'msg': '充值成功', 'data': {'id': 1115509, 'leaveamount': '49392.00', 'type': '1', 'pwd': 'F1887D3F9E6EE7A32FE5E76F4AB80D63', 'mobilephone': '17751810001', 'regname': 'å¤\x9cé\x9b¨å£°ç\x83¦', 'regtime': '2019-01-21 10:30:31.0'}, 'code': '10001'}</t>
   </si>
   <si>
+    <t>不登录直接取现</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>/member/withdraw</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":"5"}</t>
+  </si>
+  <si>
+    <t>{'status': 0, 'data': None, 'code': None, 'msg': '抱歉，请先登录。'}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '抱歉，请先登录。', 'code': None}</t>
+  </si>
+  <si>
+    <t>正常登录后取现(余额充足)</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","pwd":"123456"}</t>
+  </si>
+  <si>
+    <t>{'status': 1, 'code': '10001', 'msg': '取现成功', 'data': {'type': '1','mobilephone':'17751810779'}}</t>
+  </si>
+  <si>
+    <t>{'data': {'regname': '小蜜蜂', 'id': 1115661, 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'leaveamount': '499775.00', 'mobilephone': '17751810779', 'type': '1', 'regtime': '2019-01-21 18:01:06.0'}, 'status': 1, 'msg': '取现成功', 'code': '10001'}</t>
+  </si>
+  <si>
+    <t>{"mobilephone":None,"amount":"5"}</t>
+  </si>
+  <si>
+    <t>{'msg': '手机号不能为空', 'status': 0, 'code': '20103', 'data': None}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '手机号不能为空', 'code': '20103'}</t>
+  </si>
+  <si>
+    <t>取现金额为空</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":None}</t>
+  </si>
+  <si>
+    <t>{'msg': '请输入金额', 'status': 0, 'code': '20115', 'data': None}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '请输入金额', 'code': '20115'}</t>
+  </si>
+  <si>
+    <t>取现的手机号码不存在</t>
+  </si>
+  <si>
+    <t>{"mobilephone": "13000001403", "amount": "5"}</t>
+  </si>
+  <si>
+    <t>{'status': 1, 'code': '20104', 'data': None, 'msg': '此手机号对应的会员不存在'}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 1, 'msg': '此手机号对应的会员不存在', 'code': '20104'}</t>
+  </si>
+  <si>
+    <t>{"mobilephone": "1300s0001403", "amount": "5"}</t>
+  </si>
+  <si>
+    <t>{'code': '20109', 'data': None, 'msg': '手机号码格式不正确', 'status': 0}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '手机号码格式不正确', 'code': '20109'}</t>
+  </si>
+  <si>
+    <t>取现金额小数点大于2位</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":"0.011"}</t>
+  </si>
+  <si>
+    <t>{'status': 0, 'code': '20116', 'data': None, 'msg': '输入金额的金额小数不能超过两位'}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '输入金额的金额小数不能超过两位', 'code': '20116'}</t>
+  </si>
+  <si>
+    <t>取现金额为负数</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":"-50"}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '请输入范围在0到50万之间的正数金额', 'code': '20117'}</t>
+  </si>
+  <si>
+    <t>取现金额大于50万</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":"500001"}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'msg': '请输入范围在0到50万之间的正数金额', 'code': '20117', 'status': 0}</t>
+  </si>
+  <si>
+    <t>取现金额非数字</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":"ssss"}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 0, 'msg': '请输入数字', 'code': '20118'}</t>
+  </si>
+  <si>
+    <t>取现余额不足</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"17751810779","amount":"500000"}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'code': '20119', 'status': 1, 'msg': '余额不足，请修改提现额度'}</t>
+  </si>
+  <si>
+    <t>{'data': None, 'status': 1, 'msg': '余额不足，请修改提现额度', 'code': '20119'}</t>
+  </si>
+  <si>
+    <t>{'data': {'regname': '小蜜蜂', 'id': 1115661, 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'leaveamount': '499770.00', 'mobilephone': '17751810779', 'type': '1', 'regtime': '2019-01-21 18:01:06.0'}, 'status': 1, 'msg': '取现成功', 'code': '10001'}</t>
+  </si>
+  <si>
     <t>${mobile}</t>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>/member/withdraw</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","pwd":"123456"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":"5"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>不登录直接取现</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>正常登录后取现</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>余额充足</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'status': 1, 'code': '10001', 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>取现成功</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>', 'data': {'type': '1','mobilephone':'17751810779'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>}}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号码为空</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现金额为空</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":null,"amount":"5"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>手机号不能为空</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>', 'status': 0, 'code': '20103', 'data': None}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'status': 0, 'data': None, 'code': None, 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>抱歉，请先登录。</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>'}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>请输入金额</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>', 'status': 0, 'code': '20115', 'data': None}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":null}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'status': 1, 'code': '20104', 'data': None, 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>此手机号对应的会员不存在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>'}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现的手机号码不存在</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号码格式不正确</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone": "13000001403", "amount": "5"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'code': '20109', 'data': None, 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>手机号码格式不正确</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>', 'status': 0}</t>
-    </r>
-  </si>
-  <si>
-    <t>{"mobilephone": "1300s0001403", "amount": "5"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现金额小数点大于2位</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":"0.011"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'status': 0, 'code': '20116', 'data': None, 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>输入金额的金额小数不能超过两位</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>'}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现金额为负数</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'data': None, 'status': 0, 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>请输入范围在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>到</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>万之间的正数金额</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>', 'code': '20117'}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":"-50"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现金额大于50万</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":"500001"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{'data': None, 'msg': '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>请输入范围在</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>到</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>万之间的正数金额</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>', 'code': '20117', 'status': 0}</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现金额非数字</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":"ssss"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>取现余额不足</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"mobilephone":"17751810779","amount":"500000"}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'data': None, 'status': 0, 'msg': '请输入数字', 'code': '20118'}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'data': None, 'code': '20119', 'status': 1, 'msg': '余额不足，请修改提现额度'}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'data': None, 'status': 0, 'msg': '请输入数字', 'code': '20118'}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'data': None, 'code': '20119', 'status': 1, 'msg': '余额不足，请修改提现额度'}</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="13">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <color theme="10"/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
       <family val="3"/>
-      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -954,70 +559,61 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="8" name="超链接" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -1307,24 +903,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.625" style="1" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" style="1" width="21"/>
+    <col customWidth="1" max="4" min="4" style="1" width="30.375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="40.25"/>
+    <col customWidth="1" max="6" min="6" style="1" width="24.75"/>
+    <col customWidth="1" max="7" min="7" style="1" width="25.125"/>
+    <col customWidth="1" max="8" min="8" style="1" width="18.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="14.25" r="1" s="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1350,8 +950,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5">
+    <row customHeight="1" ht="48.75" r="2" s="1" spans="1:8">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1376,8 +976,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+    <row customHeight="1" ht="40.5" r="3" s="1" spans="1:8">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1402,8 +1002,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+    <row customHeight="1" ht="40.5" r="4" s="1" spans="1:8">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1428,8 +1028,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
+    <row customHeight="1" ht="40.5" r="5" s="1" spans="1:8">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1454,8 +1054,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row customHeight="1" ht="40.5" r="6" s="1" spans="1:8">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1480,8 +1080,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
+    <row customHeight="1" ht="40.5" r="7" s="1" spans="1:8">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1506,8 +1106,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
+    <row customHeight="1" ht="45" r="8" s="1" spans="1:8">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1532,8 +1132,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+    <row customHeight="1" ht="40.5" r="9" s="1" spans="1:8">
+      <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1558,8 +1158,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5">
+    <row customHeight="1" ht="40.5" r="10" s="1" spans="1:8">
+      <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1584,8 +1184,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5">
+    <row customHeight="1" ht="40.5" r="11" s="1" spans="1:8">
+      <c r="A11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1610,8 +1210,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
+    <row customHeight="1" ht="40.5" r="12" s="1" spans="1:8">
+      <c r="A12" s="5" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1636,8 +1236,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5">
+    <row customHeight="1" ht="40.5" r="13" s="1" spans="1:8">
+      <c r="A13" s="5" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1662,8 +1262,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
+    <row customHeight="1" ht="40.5" r="14" s="1" spans="1:8">
+      <c r="A14" s="5" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1688,8 +1288,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="5">
+    <row customHeight="1" ht="40.5" r="15" s="1" spans="1:8">
+      <c r="A15" s="5" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1714,8 +1314,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="5">
+    <row customHeight="1" ht="40.5" r="16" s="1" spans="1:8">
+      <c r="A16" s="5" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1740,8 +1340,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="5">
+    <row customHeight="1" ht="45" r="17" s="1" spans="1:8">
+      <c r="A17" s="5" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1766,8 +1366,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="5">
+    <row customHeight="1" ht="40.5" r="18" s="1" spans="1:8">
+      <c r="A18" s="5" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1792,8 +1392,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5">
+    <row customHeight="1" ht="40.5" r="19" s="1" spans="1:8">
+      <c r="A19" s="5" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1819,33 +1419,36 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://47.107.168.87:8080/futureloan/mvc/api/member/register"/>
+    <hyperlink display="http://47.107.168.87:8080/futureloan/mvc/api/member/register" ref="D2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.5" style="1" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" style="1" width="19"/>
+    <col customWidth="1" max="4" min="4" style="1" width="41.625"/>
+    <col customWidth="1" max="5" min="5" style="1" width="30.875"/>
+    <col customWidth="1" max="6" min="6" style="1" width="52.875"/>
+    <col customWidth="1" max="7" min="7" style="1" width="46.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="14.25" r="1" s="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1871,8 +1474,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
+    <row customHeight="1" ht="42.75" r="2" s="1" spans="1:8">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1897,8 +1500,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
+    <row customHeight="1" ht="30" r="3" s="1" spans="1:8">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1923,8 +1526,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+    <row customHeight="1" ht="30" r="4" s="1" spans="1:8">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1949,8 +1552,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
+    <row customHeight="1" ht="30" r="5" s="1" spans="1:8">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1975,8 +1578,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
+    <row customHeight="1" ht="30" r="6" s="1" spans="1:8">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -2001,8 +1604,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
+    <row customHeight="1" ht="30" r="7" s="1" spans="1:8">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2027,8 +1630,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
+    <row customHeight="1" ht="30" r="8" s="1" spans="1:8">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -2053,8 +1656,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
+    <row customHeight="1" ht="30" r="9" s="1" spans="1:8">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2079,8 +1682,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
+    <row customHeight="1" ht="30" r="10" s="1" spans="1:8">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2105,8 +1708,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
+    <row customHeight="1" ht="30" r="11" s="1" spans="1:8">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2132,32 +1735,35 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="44.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="56.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.75" style="1" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" style="1" width="22.5"/>
+    <col customWidth="1" max="4" min="4" style="1" width="28.375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="29.875"/>
+    <col customWidth="1" max="6" min="6" style="10" width="29.125"/>
+    <col customWidth="1" max="7" min="7" style="1" width="44.125"/>
+    <col customWidth="1" max="8" min="8" style="1" width="56.75"/>
+    <col customWidth="1" max="9" min="9" style="1" width="27.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="14.25" r="1" s="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2189,8 +1795,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
+    <row customHeight="1" ht="66" r="2" s="1" spans="1:10">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2221,8 +1827,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
+    <row customHeight="1" ht="90" r="3" s="1" spans="1:10">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2253,8 +1859,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+    <row customHeight="1" ht="30" r="4" s="1" spans="1:10">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2285,8 +1891,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
+    <row customHeight="1" ht="30" r="5" s="1" spans="1:10">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2317,8 +1923,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
+    <row customHeight="1" ht="105" r="6" s="1" spans="1:10">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2349,8 +1955,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
+    <row customHeight="1" ht="30" r="7" s="1" spans="1:10">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2381,8 +1987,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
+    <row customHeight="1" ht="40.5" r="8" s="1" spans="1:10">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -2413,8 +2019,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
+    <row customHeight="1" ht="30" r="9" s="1" spans="1:10">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2445,8 +2051,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
+    <row customHeight="1" ht="30" r="10" s="1" spans="1:10">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2477,8 +2083,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
+    <row customHeight="1" ht="30" r="11" s="1" spans="1:10">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2509,8 +2115,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
+    <row customHeight="1" ht="90" r="12" s="1" spans="1:10">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2541,8 +2147,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
+    <row customHeight="1" ht="49.5" r="13" s="1" spans="1:10">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2573,8 +2179,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
+    <row customHeight="1" ht="30" r="14" s="1" spans="1:10">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2605,8 +2211,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="3">
+    <row customHeight="1" ht="30" r="15" s="1" spans="1:10">
+      <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2637,8 +2243,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="3">
+    <row customHeight="1" ht="68.25" r="16" s="1" spans="1:10">
+      <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2669,8 +2275,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="3">
+    <row customHeight="1" ht="30" r="17" s="1" spans="1:10">
+      <c r="A17" s="3" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2701,8 +2307,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="3">
+    <row customHeight="1" ht="40.5" r="18" s="1" spans="1:10">
+      <c r="A18" s="3" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -2733,8 +2339,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="3">
+    <row customHeight="1" ht="30" r="19" s="1" spans="1:10">
+      <c r="A19" s="3" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -2765,8 +2371,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="3">
+    <row customHeight="1" ht="30" r="20" s="1" spans="1:10">
+      <c r="A20" s="3" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2797,8 +2403,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="3">
+    <row customHeight="1" ht="30" r="21" s="1" spans="1:10">
+      <c r="A21" s="3" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -2830,33 +2436,37 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
-    <col min="5" max="5" width="24.375" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="32.625" customWidth="1"/>
-    <col min="8" max="8" width="28.875" customWidth="1"/>
-    <col min="10" max="10" width="11.875" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.75"/>
+    <col customWidth="1" max="2" min="2" style="1" width="23.875"/>
+    <col customWidth="1" max="4" min="4" style="1" width="14.875"/>
+    <col customWidth="1" max="5" min="5" style="1" width="24.375"/>
+    <col customWidth="1" max="6" min="6" style="1" width="17.5"/>
+    <col customWidth="1" max="7" min="7" style="1" width="32.625"/>
+    <col customWidth="1" max="8" min="8" style="1" width="28.875"/>
+    <col customWidth="1" max="9" min="9" style="1" width="26.375"/>
+    <col customWidth="1" max="10" min="10" style="1" width="11.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customFormat="1" customHeight="1" ht="30.75" r="1" s="12" spans="1:10">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2888,161 +2498,181 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
+    <row customHeight="1" ht="30" r="2" s="1" spans="1:10">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
+      <c r="I2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="60" r="3" s="1" spans="1:10">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+      <c r="I3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="4" s="1" spans="1:10">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="5" s="1" spans="1:10">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
+      <c r="I5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="6" s="1" spans="1:10">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G6" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
+      <c r="I6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="7" s="1" spans="1:10">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>99</v>
@@ -3051,298 +2681,350 @@
         <v>118</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
+        <v>119</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="8" s="1" spans="1:10">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
+        <v>123</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="9" s="1" spans="1:10">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
+        <v>127</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="10" s="1" spans="1:10">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A11" s="6">
+      <c r="J10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="11" s="1" spans="1:10">
+      <c r="A11" s="6" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
+        <v>133</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="12" s="1" spans="1:10">
+      <c r="A12" s="6" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
+      <c r="J12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="13" s="1" spans="1:10">
+      <c r="A13" s="6" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="I13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="60" r="14" s="1" spans="1:10">
+      <c r="A14" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="I14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="15" s="1" spans="1:10">
+      <c r="A15" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="16" s="1" spans="1:10">
+      <c r="A16" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="I16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="17" s="1" spans="1:10">
+      <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G17" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="I17" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="18" s="1" spans="1:10">
+      <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>99</v>
@@ -3351,196 +3033,244 @@
         <v>118</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A19">
+        <v>119</v>
+      </c>
+      <c r="I18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="19" s="1" spans="1:10">
+      <c r="A19" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A20">
+        <v>123</v>
+      </c>
+      <c r="I19" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="20" s="1" spans="1:10">
+      <c r="A20" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A21">
+        <v>127</v>
+      </c>
+      <c r="I20" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="21" s="1" spans="1:10">
+      <c r="A21" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H21" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="22" s="1" spans="1:10">
+      <c r="A22" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" t="s">
+        <v>133</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="23" s="1" spans="1:10">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="I23" t="s">
+        <v>137</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="10.25"/>
+    <col customWidth="1" max="2" min="2" style="1" width="12.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1">
+        <v>139</v>
+      </c>
+      <c r="B1" t="n">
         <v>17751810578</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add some code in testcase
</commit_message>
<xml_diff>
--- a/datas/user_test.xlsx
+++ b/datas/user_test.xlsx
@@ -196,7 +196,7 @@
     <t>{"code":"10001", "msg":"充值成功", "data":{"type":"1", "mobilephone":"17751810000"}, "status":1}</t>
   </si>
   <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '75549.00', 'type': '1', 'mobilephone': '17751810000'}, 'msg': '充值成功', 'status': 1}</t>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810000', 'type': '1', 'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '79553.00'}, 'msg': '充值成功', 'status': 1}</t>
   </si>
   <si>
     <t>获取非本人cookie，然后正常充值</t>
@@ -211,7 +211,7 @@
     <t>{"status":1, "msg":"充值成功", "code":"10001", "data":{"mobilephone":"17751810000", "type":"1"}}</t>
   </si>
   <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '76050.00', 'type': '1', 'mobilephone': '17751810000'}, 'msg': '充值成功', 'status': 1}</t>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810000', 'type': '1', 'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '80054.00'}, 'msg': '充值成功', 'status': 1}</t>
   </si>
   <si>
     <t>获取正确cookie,手机号为空</t>
@@ -247,7 +247,7 @@
     <t>{"msg":"充值成功", "code":"10001", "data":{ "type":"1",  "mobilephone":"17751810001"}, "status":1}</t>
   </si>
   <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 10:30:31.0', 'pwd': 'F1887D3F9E6EE7A32FE5E76F4AB80D63', 'id': 1115509, 'regname': 'å¤\x9cé\x9b¨å£°ç\x83¦', 'leaveamount': '50904.00', 'type': '1', 'mobilephone': '17751810001'}, 'msg': '充值成功', 'status': 1}</t>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810001', 'type': '1', 'regtime': '2019-01-21 10:30:31.0', 'pwd': 'F1887D3F9E6EE7A32FE5E76F4AB80D63', 'id': 1115509, 'regname': 'å¤\x9cé\x9b¨å£°ç\x83¦', 'leaveamount': '52920.00'}, 'msg': '充值成功', 'status': 1}</t>
   </si>
   <si>
     <t>获取正确cookie,号码参数格式不正确</t>
@@ -304,13 +304,13 @@
     <t>{'code': '20118', 'data': None, 'msg': '请输入数字', 'status': 0}</t>
   </si>
   <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '76550.00', 'type': '1', 'mobilephone': '17751810000'}, 'msg': '充值成功', 'status': 1}</t>
-  </si>
-  <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '77051.00', 'type': '1', 'mobilephone': '17751810000'}, 'msg': '充值成功', 'status': 1}</t>
-  </si>
-  <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 10:30:31.0', 'pwd': 'F1887D3F9E6EE7A32FE5E76F4AB80D63', 'id': 1115509, 'regname': 'å¤\x9cé\x9b¨å£°ç\x83¦', 'leaveamount': '51408.00', 'type': '1', 'mobilephone': '17751810001'}, 'msg': '充值成功', 'status': 1}</t>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810000', 'type': '1', 'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '80554.00'}, 'msg': '充值成功', 'status': 1}</t>
+  </si>
+  <si>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810000', 'type': '1', 'regtime': '2019-01-21 10:35:36.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115516, 'regname': '小蜜蜂', 'leaveamount': '81055.00'}, 'msg': '充值成功', 'status': 1}</t>
+  </si>
+  <si>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810001', 'type': '1', 'regtime': '2019-01-21 10:30:31.0', 'pwd': 'F1887D3F9E6EE7A32FE5E76F4AB80D63', 'id': 1115509, 'regname': 'å¤\x9cé\x9b¨å£°ç\x83¦', 'leaveamount': '53424.00'}, 'msg': '充值成功', 'status': 1}</t>
   </si>
   <si>
     <t>不登录直接取现</t>
@@ -340,7 +340,7 @@
     <t>{'status': 1, 'code': '10001', 'msg': '取现成功', 'data': {'type': '1','mobilephone':'17751810779'}}</t>
   </si>
   <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 18:01:06.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115661, 'regname': '小蜜蜂', 'leaveamount': '499755.00', 'type': '1', 'mobilephone': '17751810779'}, 'msg': '取现成功', 'status': 1}</t>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810779', 'type': '1', 'regtime': '2019-01-21 18:01:06.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115661, 'regname': '小蜜蜂', 'leaveamount': '499735.00'}, 'msg': '取现成功', 'status': 1}</t>
   </si>
   <si>
     <t>{"mobilephone":None,"amount":"5"}</t>
@@ -421,7 +421,7 @@
     <t>{'code': '20119', 'data': None, 'msg': '余额不足，请修改提现额度', 'status': 1}</t>
   </si>
   <si>
-    <t>{'code': '10001', 'data': {'regtime': '2019-01-21 18:01:06.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115661, 'regname': '小蜜蜂', 'leaveamount': '499750.00', 'type': '1', 'mobilephone': '17751810779'}, 'msg': '取现成功', 'status': 1}</t>
+    <t>{'code': '10001', 'data': {'mobilephone': '17751810779', 'type': '1', 'regtime': '2019-01-21 18:01:06.0', 'pwd': 'E10ADC3949BA59ABBE56E057F20F883E', 'id': 1115661, 'regname': '小蜜蜂', 'leaveamount': '499730.00'}, 'msg': '取现成功', 'status': 1}</t>
   </si>
   <si>
     <t>${mobile}</t>

</xml_diff>